<commit_message>
included new stability criterion share_hybrid
</commit_message>
<xml_diff>
--- a/simulation_results/inputs/input_template_excel.xlsx
+++ b/simulation_results/inputs/input_template_excel.xlsx
@@ -673,7 +673,7 @@
     <t xml:space="preserve">stability_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve"> False or share_usage or share_backup</t>
+    <t xml:space="preserve"> False or share_usage or share_backup or share_hybrid</t>
   </si>
   <si>
     <t xml:space="preserve">renewable_constraint</t>
@@ -1231,10 +1231,9 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6428571428571"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,9 +1450,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,11 +1915,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,9 +2693,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2738,12 +2732,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,16 +2832,14 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3188,10 +3178,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>